<commit_message>
Code van week 2
Code van week 2
</commit_message>
<xml_diff>
--- a/animalchange/databron/Aantal inwonders per provincie.xlsx
+++ b/animalchange/databron/Aantal inwonders per provincie.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db9e4f8f00016419/Documenten/Data Processing/Homework/Week_7/databron/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobbo\OneDrive\Documenten\GitHub\Programmeerproject\animalchange\databron\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="BB00F7D41A4F1D112F2968F6F235AE6FF0E48C1E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{587953D9-C6CB-4668-9E0E-AAA3B196E14E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="215">
   <si>
     <t/>
   </si>
@@ -673,7 +674,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -731,9 +732,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1049,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:HR222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="HH1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:HR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1063,7 @@
     <col min="3" max="3" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1072,8 +1073,674 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CV1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DD1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DG1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DH1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DI1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DJ1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DK1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DL1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DM1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DN1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DO1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DP1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DQ1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DR1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DS1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DT1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="DU1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DV1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DW1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DX1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DY1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DZ1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EA1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EB1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EC1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="ED1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EE1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EG1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EH1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EI1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EJ1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EK1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="EL1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EM1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EN1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EO1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EP1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EQ1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="ER1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="ES1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="ET1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EU1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EV1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EW1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EX1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EY1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="EZ1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="FA1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="FB1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="FC1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FD1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FE1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FF1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FG1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FI1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FJ1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FK1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FL1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FM1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FN1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FO1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FP1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FQ1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FR1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FS1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="FT1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FU1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FV1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FW1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FX1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FY1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="FZ1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GA1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GB1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GC1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GD1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GE1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GF1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GG1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GH1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GJ1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="GK1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GL1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GM1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GN1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GO1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GP1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GQ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GR1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GS1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GT1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GU1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GV1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GW1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GX1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GY1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="GZ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="HA1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="HB1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HC1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HD1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HE1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HF1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HG1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HH1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HI1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HJ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HK1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HL1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HM1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HN1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HO1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HP1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HQ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HR1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1083,8 +1750,674 @@
       <c r="C2" s="5">
         <v>15863950</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BU2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BV2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="BW2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="CF2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CH2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="CI2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="CJ2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="CL2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="CN2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="CO2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="CR2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="CS2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="CU2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="CV2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="CW2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="CX2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CY2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="DA2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="DB2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="DE2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="DF2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DG2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="DH2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="DI2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="DJ2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="DK2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="DL2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="DM2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="DO2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="DP2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="DQ2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="DR2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="DS2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="DT2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="DU2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="DV2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DX2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="DY2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="DZ2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="EA2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="EB2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="EC2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="ED2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="EE2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="EF2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="EG2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="EH2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="EI2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="EJ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="EK2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="EL2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="EM2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="EN2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="EO2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="EP2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="EQ2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="ER2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="ES2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="ET2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="EU2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="EV2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="EW2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="EX2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="EY2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="EZ2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="FA2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="FB2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="FC2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="FD2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="FE2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="FF2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="FG2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="FH2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="FI2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="FJ2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="FK2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="FL2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="FM2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="FN2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="FO2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="FP2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="FQ2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="FR2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="FS2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="FT2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="FU2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="FV2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="FW2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="FX2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="FY2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="FZ2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="GA2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="GB2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="GC2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="GD2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="GE2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="GF2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="GG2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="GH2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="GI2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="GJ2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="GK2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="GL2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="GM2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="GN2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="GO2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="GP2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="GQ2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="GR2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="GS2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="GT2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="GU2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="GV2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="GW2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="GX2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="GY2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="GZ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="HA2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="HB2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="HC2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="HD2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="HE2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="HF2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="HG2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="HH2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="HI2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="HJ2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="HK2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="HL2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="HM2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="HN2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="HO2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="HP2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="HQ2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="HR2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1094,8 +2427,674 @@
       <c r="C3" s="5">
         <v>15987075</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5">
+        <v>15863950</v>
+      </c>
+      <c r="G3" s="5">
+        <v>15987075</v>
+      </c>
+      <c r="H3" s="5">
+        <v>16105285</v>
+      </c>
+      <c r="I3" s="5">
+        <v>16192572</v>
+      </c>
+      <c r="J3" s="5">
+        <v>16258032</v>
+      </c>
+      <c r="K3" s="5">
+        <v>16305526</v>
+      </c>
+      <c r="L3" s="5">
+        <v>16334210</v>
+      </c>
+      <c r="M3" s="5">
+        <v>16357992</v>
+      </c>
+      <c r="N3" s="5">
+        <v>16405399</v>
+      </c>
+      <c r="O3" s="5">
+        <v>16485787</v>
+      </c>
+      <c r="P3" s="5">
+        <v>16574989</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>16655799</v>
+      </c>
+      <c r="R3" s="5">
+        <v>16730348</v>
+      </c>
+      <c r="S3" s="5">
+        <v>16779575</v>
+      </c>
+      <c r="T3" s="5">
+        <v>16829289</v>
+      </c>
+      <c r="U3" s="5">
+        <v>16900726</v>
+      </c>
+      <c r="V3" s="5">
+        <v>16979120</v>
+      </c>
+      <c r="W3" s="5">
+        <v>562646</v>
+      </c>
+      <c r="X3" s="5">
+        <v>566489</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>570480</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>572997</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>574384</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>575072</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>574042</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>573614</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>573459</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>574092</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>576668</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>579036</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>580875</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>581705</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>582728</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>583942</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>583721</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>624500</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>630539</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>636184</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>639787</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>642066</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>642977</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>642230</v>
+      </c>
+      <c r="AU3" s="5">
+        <v>642209</v>
+      </c>
+      <c r="AV3" s="5">
+        <v>643189</v>
+      </c>
+      <c r="AW3" s="5">
+        <v>644811</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>646305</v>
+      </c>
+      <c r="AY3" s="5">
+        <v>647282</v>
+      </c>
+      <c r="AZ3" s="5">
+        <v>647214</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>646862</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>646317</v>
+      </c>
+      <c r="BC3" s="5">
+        <v>646257</v>
+      </c>
+      <c r="BD3" s="5">
+        <v>646040</v>
+      </c>
+      <c r="BE3" s="5">
+        <v>469806</v>
+      </c>
+      <c r="BF3" s="5">
+        <v>474506</v>
+      </c>
+      <c r="BG3" s="5">
+        <v>478799</v>
+      </c>
+      <c r="BH3" s="5">
+        <v>481254</v>
+      </c>
+      <c r="BI3" s="5">
+        <v>482415</v>
+      </c>
+      <c r="BJ3" s="5">
+        <v>483369</v>
+      </c>
+      <c r="BK3" s="5">
+        <v>484481</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>486197</v>
+      </c>
+      <c r="BM3" s="5">
+        <v>488135</v>
+      </c>
+      <c r="BN3" s="5">
+        <v>489918</v>
+      </c>
+      <c r="BO3" s="5">
+        <v>490981</v>
+      </c>
+      <c r="BP3" s="5">
+        <v>491411</v>
+      </c>
+      <c r="BQ3" s="5">
+        <v>490807</v>
+      </c>
+      <c r="BR3" s="5">
+        <v>489918</v>
+      </c>
+      <c r="BS3" s="5">
+        <v>488988</v>
+      </c>
+      <c r="BT3" s="5">
+        <v>488576</v>
+      </c>
+      <c r="BU3" s="5">
+        <v>488629</v>
+      </c>
+      <c r="BV3" s="5">
+        <v>1077625</v>
+      </c>
+      <c r="BW3" s="5">
+        <v>1086280</v>
+      </c>
+      <c r="BX3" s="5">
+        <v>1094032</v>
+      </c>
+      <c r="BY3" s="5">
+        <v>1100677</v>
+      </c>
+      <c r="BZ3" s="5">
+        <v>1105512</v>
+      </c>
+      <c r="CA3" s="5">
+        <v>1109432</v>
+      </c>
+      <c r="CB3" s="5">
+        <v>1113529</v>
+      </c>
+      <c r="CC3" s="5">
+        <v>1116374</v>
+      </c>
+      <c r="CD3" s="5">
+        <v>1119994</v>
+      </c>
+      <c r="CE3" s="5">
+        <v>1125435</v>
+      </c>
+      <c r="CF3" s="5">
+        <v>1130345</v>
+      </c>
+      <c r="CG3" s="5">
+        <v>1134465</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>1137668</v>
+      </c>
+      <c r="CI3" s="5">
+        <v>1139350</v>
+      </c>
+      <c r="CJ3" s="5">
+        <v>1139697</v>
+      </c>
+      <c r="CK3" s="5">
+        <v>1140652</v>
+      </c>
+      <c r="CL3" s="5">
+        <v>1144280</v>
+      </c>
+      <c r="CM3" s="5">
+        <v>317206</v>
+      </c>
+      <c r="CN3" s="5">
+        <v>328936</v>
+      </c>
+      <c r="CO3" s="5">
+        <v>341721</v>
+      </c>
+      <c r="CP3" s="5">
+        <v>351680</v>
+      </c>
+      <c r="CQ3" s="5">
+        <v>359904</v>
+      </c>
+      <c r="CR3" s="5">
+        <v>365859</v>
+      </c>
+      <c r="CS3" s="5">
+        <v>370656</v>
+      </c>
+      <c r="CT3" s="5">
+        <v>374424</v>
+      </c>
+      <c r="CU3" s="5">
+        <v>378688</v>
+      </c>
+      <c r="CV3" s="5">
+        <v>383449</v>
+      </c>
+      <c r="CW3" s="5">
+        <v>387881</v>
+      </c>
+      <c r="CX3" s="5">
+        <v>391967</v>
+      </c>
+      <c r="CY3" s="5">
+        <v>395525</v>
+      </c>
+      <c r="CZ3" s="5">
+        <v>398441</v>
+      </c>
+      <c r="DA3" s="5">
+        <v>399893</v>
+      </c>
+      <c r="DB3" s="5">
+        <v>401791</v>
+      </c>
+      <c r="DC3" s="5">
+        <v>404068</v>
+      </c>
+      <c r="DD3" s="5">
+        <v>1919158</v>
+      </c>
+      <c r="DE3" s="5">
+        <v>1934314</v>
+      </c>
+      <c r="DF3" s="5">
+        <v>1949233</v>
+      </c>
+      <c r="DG3" s="5">
+        <v>1960422</v>
+      </c>
+      <c r="DH3" s="5">
+        <v>1966929</v>
+      </c>
+      <c r="DI3" s="5">
+        <v>1972010</v>
+      </c>
+      <c r="DJ3" s="5">
+        <v>1975704</v>
+      </c>
+      <c r="DK3" s="5">
+        <v>1979059</v>
+      </c>
+      <c r="DL3" s="5">
+        <v>1983869</v>
+      </c>
+      <c r="DM3" s="5">
+        <v>1991062</v>
+      </c>
+      <c r="DN3" s="5">
+        <v>1998936</v>
+      </c>
+      <c r="DO3" s="5">
+        <v>2004671</v>
+      </c>
+      <c r="DP3" s="5">
+        <v>2010745</v>
+      </c>
+      <c r="DQ3" s="5">
+        <v>2015791</v>
+      </c>
+      <c r="DR3" s="5">
+        <v>2019692</v>
+      </c>
+      <c r="DS3" s="5">
+        <v>2026578</v>
+      </c>
+      <c r="DT3" s="5">
+        <v>2035351</v>
+      </c>
+      <c r="DU3" s="5">
+        <v>1107849</v>
+      </c>
+      <c r="DV3" s="5">
+        <v>1117997</v>
+      </c>
+      <c r="DW3" s="5">
+        <v>1139925</v>
+      </c>
+      <c r="DX3" s="5">
+        <v>1152218</v>
+      </c>
+      <c r="DY3" s="5">
+        <v>1162258</v>
+      </c>
+      <c r="DZ3" s="5">
+        <v>1171291</v>
+      </c>
+      <c r="EA3" s="5">
+        <v>1180039</v>
+      </c>
+      <c r="EB3" s="5">
+        <v>1190604</v>
+      </c>
+      <c r="EC3" s="5">
+        <v>1201350</v>
+      </c>
+      <c r="ED3" s="5">
+        <v>1210869</v>
+      </c>
+      <c r="EE3" s="5">
+        <v>1220910</v>
+      </c>
+      <c r="EF3" s="5">
+        <v>1228794</v>
+      </c>
+      <c r="EG3" s="5">
+        <v>1237117</v>
+      </c>
+      <c r="EH3" s="5">
+        <v>1245294</v>
+      </c>
+      <c r="EI3" s="5">
+        <v>1253672</v>
+      </c>
+      <c r="EJ3" s="5">
+        <v>1263572</v>
+      </c>
+      <c r="EK3" s="5">
+        <v>1273613</v>
+      </c>
+      <c r="EL3" s="5">
+        <v>2518354</v>
+      </c>
+      <c r="EM3" s="5">
+        <v>2534599</v>
+      </c>
+      <c r="EN3" s="5">
+        <v>2559477</v>
+      </c>
+      <c r="EO3" s="5">
+        <v>2573120</v>
+      </c>
+      <c r="EP3" s="5">
+        <v>2587265</v>
+      </c>
+      <c r="EQ3" s="5">
+        <v>2599103</v>
+      </c>
+      <c r="ER3" s="5">
+        <v>2606584</v>
+      </c>
+      <c r="ES3" s="5">
+        <v>2613070</v>
+      </c>
+      <c r="ET3" s="5">
+        <v>2626163</v>
+      </c>
+      <c r="EU3" s="5">
+        <v>2646445</v>
+      </c>
+      <c r="EV3" s="5">
+        <v>2669084</v>
+      </c>
+      <c r="EW3" s="5">
+        <v>2691477</v>
+      </c>
+      <c r="EX3" s="5">
+        <v>2709822</v>
+      </c>
+      <c r="EY3" s="5">
+        <v>2724300</v>
+      </c>
+      <c r="EZ3" s="5">
+        <v>2741369</v>
+      </c>
+      <c r="FA3" s="5">
+        <v>2761929</v>
+      </c>
+      <c r="FB3" s="5">
+        <v>2784854</v>
+      </c>
+      <c r="FC3" s="5">
+        <v>3397744</v>
+      </c>
+      <c r="FD3" s="5">
+        <v>3420700</v>
+      </c>
+      <c r="FE3" s="5">
+        <v>3423780</v>
+      </c>
+      <c r="FF3" s="5">
+        <v>3439982</v>
+      </c>
+      <c r="FG3" s="5">
+        <v>3451942</v>
+      </c>
+      <c r="FH3" s="5">
+        <v>3458381</v>
+      </c>
+      <c r="FI3" s="5">
+        <v>3458875</v>
+      </c>
+      <c r="FJ3" s="5">
+        <v>3455097</v>
+      </c>
+      <c r="FK3" s="5">
+        <v>3461435</v>
+      </c>
+      <c r="FL3" s="5">
+        <v>3481558</v>
+      </c>
+      <c r="FM3" s="5">
+        <v>3505611</v>
+      </c>
+      <c r="FN3" s="5">
+        <v>3528324</v>
+      </c>
+      <c r="FO3" s="5">
+        <v>3552407</v>
+      </c>
+      <c r="FP3" s="5">
+        <v>3563935</v>
+      </c>
+      <c r="FQ3" s="5">
+        <v>3577032</v>
+      </c>
+      <c r="FR3" s="5">
+        <v>3600011</v>
+      </c>
+      <c r="FS3" s="5">
+        <v>3622303</v>
+      </c>
+      <c r="FT3" s="5">
+        <v>371866</v>
+      </c>
+      <c r="FU3" s="5">
+        <v>374920</v>
+      </c>
+      <c r="FV3" s="5">
+        <v>377235</v>
+      </c>
+      <c r="FW3" s="5">
+        <v>378348</v>
+      </c>
+      <c r="FX3" s="5">
+        <v>379028</v>
+      </c>
+      <c r="FY3" s="5">
+        <v>379978</v>
+      </c>
+      <c r="FZ3" s="5">
+        <v>380186</v>
+      </c>
+      <c r="GA3" s="5">
+        <v>380497</v>
+      </c>
+      <c r="GB3" s="5">
+        <v>380585</v>
+      </c>
+      <c r="GC3" s="5">
+        <v>380984</v>
+      </c>
+      <c r="GD3" s="5">
+        <v>381409</v>
+      </c>
+      <c r="GE3" s="5">
+        <v>381530</v>
+      </c>
+      <c r="GF3" s="5">
+        <v>381407</v>
+      </c>
+      <c r="GG3" s="5">
+        <v>381077</v>
+      </c>
+      <c r="GH3" s="5">
+        <v>380621</v>
+      </c>
+      <c r="GI3" s="5">
+        <v>380726</v>
+      </c>
+      <c r="GJ3" s="5">
+        <v>381252</v>
+      </c>
+      <c r="GK3" s="5">
+        <v>2356004</v>
+      </c>
+      <c r="GL3" s="5">
+        <v>2375116</v>
+      </c>
+      <c r="GM3" s="5">
+        <v>2391123</v>
+      </c>
+      <c r="GN3" s="5">
+        <v>2400198</v>
+      </c>
+      <c r="GO3" s="5">
+        <v>2406994</v>
+      </c>
+      <c r="GP3" s="5">
+        <v>2411359</v>
+      </c>
+      <c r="GQ3" s="5">
+        <v>2415946</v>
+      </c>
+      <c r="GR3" s="5">
+        <v>2419042</v>
+      </c>
+      <c r="GS3" s="5">
+        <v>2424827</v>
+      </c>
+      <c r="GT3" s="5">
+        <v>2434560</v>
+      </c>
+      <c r="GU3" s="5">
+        <v>2444158</v>
+      </c>
+      <c r="GV3" s="5">
+        <v>2454215</v>
+      </c>
+      <c r="GW3" s="5">
+        <v>2463686</v>
+      </c>
+      <c r="GX3" s="5">
+        <v>2471011</v>
+      </c>
+      <c r="GY3" s="5">
+        <v>2479274</v>
+      </c>
+      <c r="GZ3" s="5">
+        <v>2488751</v>
+      </c>
+      <c r="HA3" s="5">
+        <v>2498749</v>
+      </c>
+      <c r="HB3" s="5">
+        <v>1141192</v>
+      </c>
+      <c r="HC3" s="5">
+        <v>1142679</v>
+      </c>
+      <c r="HD3" s="5">
+        <v>1143296</v>
+      </c>
+      <c r="HE3" s="5">
+        <v>1141889</v>
+      </c>
+      <c r="HF3" s="5">
+        <v>1139335</v>
+      </c>
+      <c r="HG3" s="5">
+        <v>1136695</v>
+      </c>
+      <c r="HH3" s="5">
+        <v>1131938</v>
+      </c>
+      <c r="HI3" s="5">
+        <v>1127805</v>
+      </c>
+      <c r="HJ3" s="5">
+        <v>1123705</v>
+      </c>
+      <c r="HK3" s="5">
+        <v>1122604</v>
+      </c>
+      <c r="HL3" s="5">
+        <v>1122701</v>
+      </c>
+      <c r="HM3" s="5">
+        <v>1122627</v>
+      </c>
+      <c r="HN3" s="5">
+        <v>1123075</v>
+      </c>
+      <c r="HO3" s="5">
+        <v>1121891</v>
+      </c>
+      <c r="HP3" s="5">
+        <v>1120006</v>
+      </c>
+      <c r="HQ3" s="5">
+        <v>1117941</v>
+      </c>
+      <c r="HR3" s="5">
+        <v>1116260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +3105,7 @@
         <v>16105285</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1117,7 +3116,7 @@
         <v>16192572</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1128,7 +3127,7 @@
         <v>16258032</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +3138,7 @@
         <v>16305526</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1150,7 +3149,7 @@
         <v>16334210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +3160,7 @@
         <v>16357992</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +3171,7 @@
         <v>16405399</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +3182,7 @@
         <v>16485787</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +3193,7 @@
         <v>16574989</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +3204,7 @@
         <v>16655799</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1216,7 +3215,7 @@
         <v>16730348</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1227,7 +3226,7 @@
         <v>16779575</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:226" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>